<commit_message>
new changes to test framework
</commit_message>
<xml_diff>
--- a/src/main/java/testData/TestData_Testmanagement.xlsx
+++ b/src/main/java/testData/TestData_Testmanagement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johanlindstrom/eclipse-workspace/DataDrivenFramework/src/main/java/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BDE6B9-223D-D94D-B5B9-8CBED7E0C369}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5BD3FC-DFEE-2648-8435-40F900B61E47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24920" yWindow="2340" windowWidth="22660" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24400" yWindow="1480" windowWidth="22660" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
   <si>
     <t>Test One</t>
   </si>
@@ -221,44 +221,40 @@
     <t>Test Four</t>
   </si>
   <si>
-    <t>TD1</t>
-  </si>
-  <si>
-    <t>TD2</t>
-  </si>
-  <si>
-    <t>TD1.2</t>
-  </si>
-  <si>
-    <t>TD1.3</t>
-  </si>
-  <si>
-    <t>TD1.4</t>
-  </si>
-  <si>
-    <t>TD2.2</t>
-  </si>
-  <si>
-    <t>TD2.3</t>
-  </si>
-  <si>
-    <t>TD2.4</t>
-  </si>
-  <si>
     <t>col5</t>
   </si>
   <si>
     <t>col6</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Test1234</t>
+  </si>
+  <si>
+    <t>SDETTest@yahoo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -287,14 +283,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -607,16 +606,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -694,10 +693,10 @@
         <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -884,10 +883,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" t="s">
         <v>68</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="C27" t="s">
         <v>69</v>
@@ -896,21 +895,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" t="s">
-        <v>73</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B27" r:id="rId1" xr:uid="{C3A589B2-D5D2-3E4A-919B-75FE05E5A4BC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>